<commit_message>
Create elk detections obj
</commit_message>
<xml_diff>
--- a/data/DATABASE_Elk Capture_Updtd_20240513.xlsx
+++ b/data/DATABASE_Elk Capture_Updtd_20240513.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Databases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SPOPOV\Documents\Elk\elk-habitat\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64CC307D-0E29-4654-AF95-8F3032D2833B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF008E64-C695-4B71-81A0-A350E6877FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23832" yWindow="252" windowWidth="20988" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1170,9 +1170,6 @@
     <t>Capture_ID</t>
   </si>
   <si>
-    <t>Pimary WLH-ID</t>
-  </si>
-  <si>
     <t>Active - REDEPLOY</t>
   </si>
   <si>
@@ -1501,6 +1498,9 @@
   </si>
   <si>
     <t>RECOLLARED (22-1809R)</t>
+  </si>
+  <si>
+    <t>Primary WLH-ID</t>
   </si>
 </sst>
 </file>
@@ -1665,7 +1665,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1722,8 +1722,6 @@
     <xf numFmtId="22" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="22" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
@@ -1851,7 +1849,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{60C4E6AE-B70A-41C7-AE80-CDF76CE92A19}" type="CELLRANGE">
+                    <a:fld id="{0E2068B6-93AB-4723-85D7-2A53EF3DD03F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1884,7 +1882,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EEF60FB5-DF4D-4BC8-AC0F-7BC7933F96E4}" type="CELLRANGE">
+                    <a:fld id="{FF9D73D6-684D-43CF-BC45-9DDE9C3ED74D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1917,7 +1915,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{621500C9-81D2-4F89-9B1A-CC87A39C1709}" type="CELLRANGE">
+                    <a:fld id="{4C9836C0-129C-4532-B3BA-4873F1D50C52}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1950,7 +1948,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{194E3DFC-403D-48A2-B8B7-FD5716CA0383}" type="CELLRANGE">
+                    <a:fld id="{4B2C5DF7-F859-4F18-8B17-5003D02EC489}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1983,7 +1981,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A2175BC5-4D93-4889-B41D-56638CD1439C}" type="CELLRANGE">
+                    <a:fld id="{6C097F78-5C6A-47E2-B9A1-1F7C1A7B4CCB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2016,7 +2014,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BAEEC4FE-6A4A-4F5E-9899-7AA2BD6976AD}" type="CELLRANGE">
+                    <a:fld id="{F56C24CE-B131-48AF-B1C7-266EC0B47CB6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2049,7 +2047,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{89DB5FD1-DE0E-473F-9B08-D70AE38772ED}" type="CELLRANGE">
+                    <a:fld id="{AF62A390-0D1D-4130-BB03-38B0249AB548}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2082,7 +2080,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{47510D6A-8C42-4348-AD26-C1361B2A1207}" type="CELLRANGE">
+                    <a:fld id="{1DA90D78-4CD2-46D4-AEAD-7F3BB7F7F4FC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2115,7 +2113,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2BC6903E-D495-4153-BF44-99918CE0026B}" type="CELLRANGE">
+                    <a:fld id="{A0E9BCC8-032F-4799-9F21-D69213BAABB8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2148,7 +2146,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{929C5D26-DA43-49FB-9F61-F29CEC33FE6B}" type="CELLRANGE">
+                    <a:fld id="{C20807C4-2901-4844-9847-104CD55D2BDC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2181,7 +2179,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C7FFE74F-957C-49A0-967E-8115E3D1FB4F}" type="CELLRANGE">
+                    <a:fld id="{B650D204-870A-4154-96E5-6A3116023FFC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2214,7 +2212,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6C3E4DA7-CE35-4863-BD8B-21EAECEC6AB8}" type="CELLRANGE">
+                    <a:fld id="{096DC0AA-0B54-4A4E-9B5C-D8A4F05D93EB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2247,7 +2245,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{12F30860-FA73-4875-8153-FCCD6E9E3A4B}" type="CELLRANGE">
+                    <a:fld id="{7F50AA64-D03C-4FA7-8042-8D69894F781A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2280,7 +2278,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{76894593-BBC1-4E5E-8589-0428B9A9D6FD}" type="CELLRANGE">
+                    <a:fld id="{A3134478-49C2-4425-A949-FA217D7E0ED7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2313,7 +2311,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{135D359E-A98A-43D7-907B-0CBE027A7E49}" type="CELLRANGE">
+                    <a:fld id="{516C4324-9E99-454D-82A3-012704F178FB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2346,7 +2344,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9B96E270-C7B2-4822-8AB9-DADF77B71B96}" type="CELLRANGE">
+                    <a:fld id="{5EFC544E-7858-4EC3-B0F0-8CF41CCAF74C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2379,7 +2377,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6737F16E-8B19-4049-936C-713F5EE3C0AF}" type="CELLRANGE">
+                    <a:fld id="{52673C73-B767-4DEB-BD8C-703570ED8962}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2412,7 +2410,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0C2B74A7-75D8-47B4-9F58-67ABCA943E66}" type="CELLRANGE">
+                    <a:fld id="{75372BD0-3BE8-4923-BE07-4307DDB88018}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2445,7 +2443,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D686D7DF-E552-40F4-9DCB-AD1CBC102453}" type="CELLRANGE">
+                    <a:fld id="{A25B8E86-9047-4D9F-A5BF-C21883E36819}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2478,7 +2476,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C32B27A8-0B0A-4F5E-85A2-C3483F454DA9}" type="CELLRANGE">
+                    <a:fld id="{B682A60C-43C4-4014-9CA1-D1D9B6627EC4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2511,7 +2509,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{63EAC619-1A5C-4838-A5C6-5A3E11DDF0AE}" type="CELLRANGE">
+                    <a:fld id="{071897D3-B24E-48CD-8CFC-9CC1DC40FBFF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2544,7 +2542,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5EF5195B-D691-45C1-9AAE-1C9D90EC5566}" type="CELLRANGE">
+                    <a:fld id="{7F63B2BE-9A2C-40A2-BBBD-5FCD09C61AD6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2577,7 +2575,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8B3FA2F6-AF5C-42AF-BAE6-B23C6E8D0294}" type="CELLRANGE">
+                    <a:fld id="{EBA5C289-B977-4A4A-A77C-F27748530095}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2610,7 +2608,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9D74AE32-9EAD-4173-9130-67C9AD2DBA64}" type="CELLRANGE">
+                    <a:fld id="{6AB7FBC1-4151-4B6F-87EF-56651BE9C1BA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2643,7 +2641,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{23E09153-43F9-4F0B-9E7E-CFD1946C3B9F}" type="CELLRANGE">
+                    <a:fld id="{B4CD3306-6126-45BB-BFF7-D01ACF9D34E5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2676,7 +2674,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{85D8777C-D615-4E72-A4F5-71442DF3ED29}" type="CELLRANGE">
+                    <a:fld id="{E7157C17-6184-4DB8-B0AF-5296F596CC9B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2709,7 +2707,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BEAB0F06-4064-4835-B560-DFC0373F43F7}" type="CELLRANGE">
+                    <a:fld id="{27DC2CC0-33F5-44EE-99D7-9163A78E96D5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2742,7 +2740,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{75B12042-CDEE-4068-BFFB-C26AE5DFAE9B}" type="CELLRANGE">
+                    <a:fld id="{D273E2C8-35D9-421C-9B07-3D7FE0E78633}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2775,7 +2773,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5C3DCA4C-5750-40C9-808C-3FEB03F9C9F4}" type="CELLRANGE">
+                    <a:fld id="{F9C102AF-C67C-45F8-85D2-DB7F0B3B4280}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2808,7 +2806,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{86745861-8C35-4AAA-BD95-F0DE34F24ED9}" type="CELLRANGE">
+                    <a:fld id="{5946962A-EE96-4A17-A68A-DDA5533C6319}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2841,7 +2839,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F40F95A3-5B36-443C-8A28-8046F5E2ADA5}" type="CELLRANGE">
+                    <a:fld id="{C0A6EED2-EEE6-4264-B488-B2EB14CDAC48}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2874,7 +2872,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{223C1789-2499-437A-B5FB-71B4DEAEEF25}" type="CELLRANGE">
+                    <a:fld id="{65E85025-B557-4479-8C79-A584C0E75163}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2907,7 +2905,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6191102F-DB3B-4DED-B466-A8808C717723}" type="CELLRANGE">
+                    <a:fld id="{B08B2AE1-D86B-42CE-8C77-30BACC08645A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2940,7 +2938,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FBE8B97F-8B3D-4F7A-9015-7C1EBA28A8E0}" type="CELLRANGE">
+                    <a:fld id="{67C4F474-7DCB-465F-8ECC-B6EE2FEA6AC9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2973,7 +2971,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{61D49ED7-0058-4E58-AD68-C5A16F153330}" type="CELLRANGE">
+                    <a:fld id="{EFD5A4EC-9E32-4B19-8864-C1B71D99C435}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3006,7 +3004,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{46C46CE8-3EB6-4197-9DB2-2F9764CC58B8}" type="CELLRANGE">
+                    <a:fld id="{C288EFA0-0ADD-4769-B055-F011A3A95909}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3039,7 +3037,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AE049FDF-7E62-40A3-A2AA-A02E8C442AEC}" type="CELLRANGE">
+                    <a:fld id="{5CAE3D66-5A5E-4419-8BDC-D86BE072EA3D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3072,7 +3070,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C3E17900-A49B-42D2-9074-F4A895ADA1D2}" type="CELLRANGE">
+                    <a:fld id="{DA1DAF74-A63B-4033-96DD-2B8CF1376AB2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3105,7 +3103,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7485151F-8C2D-47FC-A032-71BA033D8C6C}" type="CELLRANGE">
+                    <a:fld id="{E5B0255C-D8C2-46AB-9B45-6A69F426F8B1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3138,7 +3136,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EF7094E2-4B91-4746-8BA7-54CE29AB358D}" type="CELLRANGE">
+                    <a:fld id="{C12B4AF0-EF4E-49D7-BFA9-6470CD5E6407}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3171,7 +3169,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8ECC8CB7-678F-4C63-9AFC-A551DD311910}" type="CELLRANGE">
+                    <a:fld id="{753642B9-D7F8-4B52-AC0C-28514BAC2A2F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3204,7 +3202,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{784055BC-6711-4C2A-B914-4BBCCD53E2FE}" type="CELLRANGE">
+                    <a:fld id="{4AC35C20-FA2B-48D6-B755-ED2DC0CD6A35}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3237,7 +3235,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{195665F4-00BE-4434-AC03-6BF5257ED017}" type="CELLRANGE">
+                    <a:fld id="{5D91C812-C2E7-4C2A-9762-8BD979FF3DAC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3270,7 +3268,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F6E9F7FA-9687-4813-925A-EBEC1C59C449}" type="CELLRANGE">
+                    <a:fld id="{E82A8D35-D689-4324-A85A-C76E444183CC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3303,7 +3301,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A161E3BC-EEB7-41C1-949F-4AEC9C1B5881}" type="CELLRANGE">
+                    <a:fld id="{263DBC4F-15B1-4BF3-9F93-C7F8231660B0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3336,7 +3334,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EE510B69-D787-4AF6-AA3E-CB9C205DD385}" type="CELLRANGE">
+                    <a:fld id="{5E5DE678-A3EB-4544-9F72-B68EB5B7D8EF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3369,7 +3367,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{362FB423-8135-4235-BA3D-6D24D037EBD2}" type="CELLRANGE">
+                    <a:fld id="{89C8ED8B-2F37-430A-8AA6-7CDD1C408655}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3402,7 +3400,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{00724D35-4314-43C5-93B3-61811BAAA1A9}" type="CELLRANGE">
+                    <a:fld id="{E885C628-BAD2-4601-8FBF-E43A537F0DE7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3435,7 +3433,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{42841378-F531-4639-9E57-7523DDC0BEF7}" type="CELLRANGE">
+                    <a:fld id="{C3776D9F-59D7-496B-9AA7-12658F03C813}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3468,7 +3466,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FE614EB4-D6D6-462C-AAEE-49A2BC7AA83B}" type="CELLRANGE">
+                    <a:fld id="{56AD0DEC-2965-4E34-AB3A-D4F97F0A0279}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3501,7 +3499,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D4662C76-2CA8-4F04-8ED0-2CF565628F26}" type="CELLRANGE">
+                    <a:fld id="{EDBA67FF-71FA-46E0-B478-08A5909A7836}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3534,7 +3532,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{91E0AF2A-EB92-496F-81BF-E49211BCE294}" type="CELLRANGE">
+                    <a:fld id="{D6F301C0-CD14-4DC4-912B-EC22FA39203F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3567,7 +3565,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4A0DE27E-0EBF-49F7-B7DE-295EBBDCFACA}" type="CELLRANGE">
+                    <a:fld id="{D1A46F5B-6D5A-4F8F-B797-8DC44C6D6800}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3600,7 +3598,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D7D8ED9B-FAE1-4B74-989C-FB978F1B1A3D}" type="CELLRANGE">
+                    <a:fld id="{BF88865F-C1C0-4107-B7EE-DB379C52B561}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3633,7 +3631,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AB8665EA-CB5A-4811-ABC8-3C3ED87BF4CD}" type="CELLRANGE">
+                    <a:fld id="{2F5FD395-F903-4696-BE84-B3D37BEBAAA8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3666,7 +3664,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5674129C-727D-417E-827B-303DE063F38A}" type="CELLRANGE">
+                    <a:fld id="{25C7309E-32A6-43BC-B4AF-748AEBA75DDF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3699,7 +3697,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{01441422-E40E-46CA-BC65-28FA0678D0DF}" type="CELLRANGE">
+                    <a:fld id="{708870C9-2C9F-42D9-985D-F9FEB8DB4058}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3732,7 +3730,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9A285556-E263-40C0-9D0E-A43F9088EF7C}" type="CELLRANGE">
+                    <a:fld id="{019DE3EB-E8F7-431C-A27C-267152CC404B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3765,7 +3763,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{150CB420-D7E7-4B9D-9208-3BCD871A9912}" type="CELLRANGE">
+                    <a:fld id="{AE542ED1-2E76-464E-ABCF-FC2D0B9D60B1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3798,7 +3796,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{531CE06F-4E71-428A-928A-88E19E75D673}" type="CELLRANGE">
+                    <a:fld id="{FA8D7E84-3DE7-474A-A4DF-DD9CC05676D0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3831,7 +3829,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A64F8766-C047-43CC-85B0-62EBB8FB8461}" type="CELLRANGE">
+                    <a:fld id="{2388B08B-42BE-4044-8691-B8D0F37D9336}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3864,7 +3862,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{50AE5F5C-7406-4F7D-8ED1-4A57D654109D}" type="CELLRANGE">
+                    <a:fld id="{51FB15AA-72F5-49E5-B647-4684F30CBAEF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3897,7 +3895,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1B7AF837-49F9-411C-A732-A5F6879C6825}" type="CELLRANGE">
+                    <a:fld id="{F237F7EC-82E4-4457-9014-6E9D9563CA19}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3930,7 +3928,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F5352762-0B3F-46DA-9F05-D5A83116DF6C}" type="CELLRANGE">
+                    <a:fld id="{C8FB3650-A6D4-4295-B236-3C338FD82B2D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3963,7 +3961,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5EBEF524-D73B-4D9C-8FCC-9A0A4E3E4151}" type="CELLRANGE">
+                    <a:fld id="{F925C072-F840-4418-A856-783223DF2021}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3996,7 +3994,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9F82A92F-102D-4705-96F1-87040638E9D7}" type="CELLRANGE">
+                    <a:fld id="{2B026EA6-C14C-4965-8A06-06227F871FAF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4029,7 +4027,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{297E6690-D081-4D23-A1D3-19D5CCC8897F}" type="CELLRANGE">
+                    <a:fld id="{0E497E24-4C99-4E36-B09A-8BD529E0A9CC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4062,7 +4060,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5B8A99C9-FE4F-4E29-A9F4-46B0E259052C}" type="CELLRANGE">
+                    <a:fld id="{5BB622B1-FFB2-47C1-894A-9898B30ACC8E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4095,7 +4093,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C4BC67D2-480D-4B20-8911-D23175D51901}" type="CELLRANGE">
+                    <a:fld id="{4D60C633-5F4E-48D6-BBB9-8B7A80A2DDF4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5972,64 +5970,64 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BD86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BC25" sqref="BC25"/>
+      <selection pane="bottomLeft" activeCell="Z1" sqref="Z1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
     <col min="4" max="4" width="6" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="18.88671875" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="5.6640625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="6.6640625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="6.5546875" style="4" customWidth="1"/>
-    <col min="11" max="11" width="7.33203125" style="4" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" style="4" customWidth="1"/>
-    <col min="13" max="13" width="10.88671875" style="4" customWidth="1"/>
-    <col min="14" max="14" width="11.5546875" style="4" customWidth="1"/>
-    <col min="15" max="15" width="9.109375" style="4" customWidth="1"/>
-    <col min="16" max="16" width="9.33203125" style="4" customWidth="1"/>
-    <col min="17" max="17" width="9.109375" style="4" customWidth="1"/>
-    <col min="18" max="18" width="11.5546875" style="4" customWidth="1"/>
-    <col min="19" max="19" width="13.5546875" style="4" customWidth="1"/>
-    <col min="20" max="20" width="16.109375" style="4" customWidth="1"/>
-    <col min="21" max="21" width="14.5546875" style="4" customWidth="1"/>
-    <col min="22" max="22" width="11.88671875" style="4" customWidth="1"/>
-    <col min="23" max="23" width="9.88671875" style="4" customWidth="1"/>
-    <col min="24" max="24" width="11.5546875" style="4" customWidth="1"/>
-    <col min="25" max="25" width="12.33203125" style="4" customWidth="1"/>
-    <col min="26" max="26" width="16.6640625" customWidth="1"/>
-    <col min="27" max="27" width="22.6640625" customWidth="1"/>
-    <col min="28" max="28" width="10.33203125" customWidth="1"/>
-    <col min="29" max="29" width="13.88671875" customWidth="1"/>
-    <col min="30" max="30" width="8.88671875" hidden="1" customWidth="1"/>
-    <col min="31" max="31" width="11.33203125" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="12.109375" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="33.33203125" hidden="1" customWidth="1"/>
-    <col min="34" max="34" width="8.88671875" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="10.88671875" hidden="1" customWidth="1"/>
-    <col min="36" max="38" width="8.88671875" hidden="1" customWidth="1"/>
-    <col min="39" max="39" width="18.5546875" hidden="1" customWidth="1"/>
-    <col min="40" max="40" width="10.33203125" hidden="1" customWidth="1"/>
-    <col min="41" max="41" width="14.6640625" hidden="1" customWidth="1"/>
-    <col min="42" max="42" width="10.88671875" style="4" hidden="1" customWidth="1"/>
-    <col min="43" max="45" width="14.6640625" style="4" hidden="1" customWidth="1"/>
-    <col min="46" max="48" width="8.88671875" style="4" hidden="1" customWidth="1"/>
-    <col min="49" max="52" width="8.88671875" hidden="1" customWidth="1"/>
-    <col min="53" max="53" width="9.6640625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="6.5703125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="7.28515625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" style="4" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="4" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="4" customWidth="1"/>
+    <col min="16" max="16" width="9.28515625" style="4" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" style="4" customWidth="1"/>
+    <col min="18" max="18" width="11.5703125" style="4" customWidth="1"/>
+    <col min="19" max="19" width="13.5703125" style="4" customWidth="1"/>
+    <col min="20" max="20" width="16.140625" style="4" customWidth="1"/>
+    <col min="21" max="21" width="14.5703125" style="4" customWidth="1"/>
+    <col min="22" max="22" width="11.85546875" style="4" customWidth="1"/>
+    <col min="23" max="23" width="9.85546875" style="4" customWidth="1"/>
+    <col min="24" max="24" width="11.5703125" style="4" customWidth="1"/>
+    <col min="25" max="25" width="12.28515625" style="4" customWidth="1"/>
+    <col min="26" max="26" width="16.7109375" customWidth="1"/>
+    <col min="27" max="27" width="22.7109375" customWidth="1"/>
+    <col min="28" max="28" width="10.28515625" customWidth="1"/>
+    <col min="29" max="29" width="13.85546875" customWidth="1"/>
+    <col min="30" max="30" width="8.85546875" hidden="1" customWidth="1"/>
+    <col min="31" max="31" width="11.28515625" hidden="1" customWidth="1"/>
+    <col min="32" max="32" width="12.140625" hidden="1" customWidth="1"/>
+    <col min="33" max="33" width="33.28515625" hidden="1" customWidth="1"/>
+    <col min="34" max="34" width="8.85546875" hidden="1" customWidth="1"/>
+    <col min="35" max="35" width="10.85546875" hidden="1" customWidth="1"/>
+    <col min="36" max="38" width="8.85546875" hidden="1" customWidth="1"/>
+    <col min="39" max="39" width="18.5703125" hidden="1" customWidth="1"/>
+    <col min="40" max="40" width="10.28515625" hidden="1" customWidth="1"/>
+    <col min="41" max="41" width="14.7109375" hidden="1" customWidth="1"/>
+    <col min="42" max="42" width="10.85546875" style="4" hidden="1" customWidth="1"/>
+    <col min="43" max="45" width="14.7109375" style="4" hidden="1" customWidth="1"/>
+    <col min="46" max="48" width="8.85546875" style="4" hidden="1" customWidth="1"/>
+    <col min="49" max="52" width="8.85546875" hidden="1" customWidth="1"/>
+    <col min="53" max="53" width="9.7109375" hidden="1" customWidth="1"/>
     <col min="54" max="54" width="30" customWidth="1"/>
-    <col min="55" max="55" width="41.6640625" customWidth="1"/>
-    <col min="56" max="56" width="124.109375" customWidth="1"/>
-    <col min="57" max="58" width="9.109375" customWidth="1"/>
+    <col min="55" max="55" width="41.7109375" customWidth="1"/>
+    <col min="56" max="56" width="124.140625" customWidth="1"/>
+    <col min="57" max="58" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:56" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>376</v>
       </c>
@@ -6106,7 +6104,7 @@
         <v>19</v>
       </c>
       <c r="Z1" s="5" t="s">
-        <v>377</v>
+        <v>487</v>
       </c>
       <c r="AA1" s="5" t="s">
         <v>21</v>
@@ -6127,7 +6125,7 @@
         <v>27</v>
       </c>
       <c r="AG1" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AH1" s="5" t="s">
         <v>30</v>
@@ -6199,12 +6197,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>467</v>
+      </c>
+      <c r="B2" t="s">
         <v>468</v>
-      </c>
-      <c r="B2" t="s">
-        <v>469</v>
       </c>
       <c r="C2" s="6">
         <v>44981</v>
@@ -6213,10 +6211,10 @@
         <v>-2</v>
       </c>
       <c r="E2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="F2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G2" s="4">
         <v>12</v>
@@ -6246,10 +6244,10 @@
         <v>3</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="R2" s="3">
         <v>0.45347222222222222</v>
@@ -6267,7 +6265,7 @@
         <v>0.4826388888888889</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="X2" s="4">
         <v>49.622909999999997</v>
@@ -6276,7 +6274,7 @@
         <v>-126.042653</v>
       </c>
       <c r="Z2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="AA2" t="s">
         <v>22</v>
@@ -6288,25 +6286,25 @@
         <v>31995</v>
       </c>
       <c r="AD2" t="s">
+        <v>471</v>
+      </c>
+      <c r="AE2" t="s">
         <v>472</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>473</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>474</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>475</v>
       </c>
       <c r="AH2" t="s">
         <v>31</v>
       </c>
       <c r="AI2" t="s">
+        <v>475</v>
+      </c>
+      <c r="AJ2" t="s">
         <v>476</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>477</v>
       </c>
       <c r="AK2" t="s">
         <v>360</v>
@@ -6366,7 +6364,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -6533,7 +6531,7 @@
         <v>44928.861192129632</v>
       </c>
     </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>80</v>
       </c>
@@ -6703,7 +6701,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -6864,7 +6862,7 @@
         <v>50</v>
       </c>
       <c r="BB5" s="35" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="BC5" s="33">
         <v>45336.958912037036</v>
@@ -6873,7 +6871,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -7036,11 +7034,11 @@
       <c r="BB6" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="BC6" s="38">
+      <c r="BC6" s="36">
         <v>44475</v>
       </c>
     </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>74</v>
       </c>
@@ -7203,14 +7201,14 @@
       <c r="BB7" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="BC7" s="38">
+      <c r="BC7" s="36">
         <v>44675</v>
       </c>
       <c r="BD7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -7373,14 +7371,14 @@
       <c r="BB8" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="BC8" s="38">
+      <c r="BC8" s="36">
         <v>44132</v>
       </c>
       <c r="BD8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>172</v>
       </c>
@@ -7541,7 +7539,7 @@
         <v>73</v>
       </c>
       <c r="BB9" s="35" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="BC9" s="33">
         <v>45185.583333333336</v>
@@ -7550,7 +7548,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -7713,14 +7711,14 @@
       <c r="BB10" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="BC10" s="38">
+      <c r="BC10" s="36">
         <v>43643</v>
       </c>
       <c r="BD10" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>104</v>
       </c>
@@ -7882,7 +7880,7 @@
         <v>50</v>
       </c>
       <c r="BB11" s="13" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="BC11" s="33">
         <v>45189.33388888889</v>
@@ -7891,7 +7889,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>151</v>
       </c>
@@ -8062,7 +8060,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="13" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>160</v>
       </c>
@@ -8230,7 +8228,7 @@
         <v>44352.834097222221</v>
       </c>
     </row>
-    <row r="14" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>90</v>
       </c>
@@ -8394,16 +8392,16 @@
       <c r="BB14" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="BC14" s="38">
+      <c r="BC14" s="36">
         <v>44816</v>
       </c>
       <c r="BD14" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B15" t="s">
         <v>232</v>
@@ -8418,7 +8416,7 @@
         <v>99</v>
       </c>
       <c r="F15" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="G15" s="4">
         <v>19</v>
@@ -8493,7 +8491,7 @@
         <v>180</v>
       </c>
       <c r="AE15" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="AF15" t="s">
         <v>329</v>
@@ -8514,7 +8512,7 @@
         <v>360</v>
       </c>
       <c r="AL15" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="AM15">
         <v>38.5</v>
@@ -8562,16 +8560,16 @@
         <v>73</v>
       </c>
       <c r="BB15" s="13" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="BC15" t="s">
         <v>270</v>
       </c>
       <c r="BD15" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
-    <row r="16" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>116</v>
       </c>
@@ -8733,16 +8731,16 @@
         <v>73</v>
       </c>
       <c r="BB16" s="35" t="s">
-        <v>435</v>
-      </c>
-      <c r="BC16" s="36">
+        <v>434</v>
+      </c>
+      <c r="BC16" s="33">
         <v>44982.959004629629</v>
       </c>
       <c r="BD16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>183</v>
       </c>
@@ -8906,16 +8904,16 @@
       <c r="BB17" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="BC17" s="38">
+      <c r="BC17" s="36">
         <v>44690</v>
       </c>
       <c r="BD17" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="18" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B18" t="s">
         <v>133</v>
@@ -8930,7 +8928,7 @@
         <v>85</v>
       </c>
       <c r="F18" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G18" s="4">
         <v>7</v>
@@ -8990,7 +8988,7 @@
         <v>-126.06818</v>
       </c>
       <c r="Z18" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="AA18" t="s">
         <v>22</v>
@@ -9005,13 +9003,13 @@
         <v>137</v>
       </c>
       <c r="AE18" t="s">
+        <v>419</v>
+      </c>
+      <c r="AF18" t="s">
         <v>420</v>
       </c>
-      <c r="AF18" t="s">
+      <c r="AG18" t="s">
         <v>421</v>
-      </c>
-      <c r="AG18" t="s">
-        <v>422</v>
       </c>
       <c r="AH18" t="s">
         <v>31</v>
@@ -9026,7 +9024,7 @@
         <v>360</v>
       </c>
       <c r="AL18" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="AM18">
         <v>38.1</v>
@@ -9076,11 +9074,11 @@
       <c r="BB18" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="BC18" s="38">
+      <c r="BC18" s="36">
         <v>45411</v>
       </c>
     </row>
-    <row r="19" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>187</v>
       </c>
@@ -9244,14 +9242,14 @@
       <c r="BB19" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="BC19" s="38">
+      <c r="BC19" s="36">
         <v>44977</v>
       </c>
       <c r="BD19" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="20" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>100</v>
       </c>
@@ -9415,11 +9413,11 @@
       <c r="BB20" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="BC20" s="36">
+      <c r="BC20" s="33">
         <v>45069.834826388891</v>
       </c>
     </row>
-    <row r="21" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>111</v>
       </c>
@@ -9583,11 +9581,11 @@
       <c r="BB21" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="BC21" s="36">
+      <c r="BC21" s="33">
         <v>45338.959050925929</v>
       </c>
     </row>
-    <row r="22" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>190</v>
       </c>
@@ -9755,7 +9753,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="23" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>136</v>
       </c>
@@ -9918,14 +9916,14 @@
       <c r="BB23" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="BC23" s="36">
+      <c r="BC23" s="33">
         <v>44240.209074074075</v>
       </c>
       <c r="BD23" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="24" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>127</v>
       </c>
@@ -10096,7 +10094,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="25" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>123</v>
       </c>
@@ -10260,14 +10258,14 @@
       <c r="BB25" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="BC25" s="38">
+      <c r="BC25" s="36">
         <v>44274</v>
       </c>
       <c r="BD25" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="26" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>120</v>
       </c>
@@ -10431,14 +10429,14 @@
       <c r="BB26" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="BC26" s="38">
+      <c r="BC26" s="36">
         <v>44642</v>
       </c>
       <c r="BD26" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>176</v>
       </c>
@@ -10601,11 +10599,11 @@
       <c r="BB27" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="BC27" s="38">
+      <c r="BC27" s="36">
         <v>45381</v>
       </c>
     </row>
-    <row r="28" spans="1:56" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:56" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>97</v>
       </c>
@@ -10774,7 +10772,7 @@
       </c>
       <c r="BD28"/>
     </row>
-    <row r="29" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>167</v>
       </c>
@@ -10945,7 +10943,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="30" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>156</v>
       </c>
@@ -11115,7 +11113,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="31" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>131</v>
       </c>
@@ -11277,13 +11275,13 @@
         <v>73</v>
       </c>
       <c r="BB31" s="13" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="BC31" s="33">
         <v>44525.333587962959</v>
       </c>
     </row>
-    <row r="32" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>164</v>
       </c>
@@ -11447,14 +11445,14 @@
       <c r="BB32" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="BC32" s="38">
+      <c r="BC32" s="36">
         <v>44289</v>
       </c>
       <c r="BD32" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="33" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>291</v>
       </c>
@@ -11615,13 +11613,13 @@
         <v>73</v>
       </c>
       <c r="BB33" s="35" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="BC33" s="33">
         <v>45012.958877314813</v>
       </c>
     </row>
-    <row r="34" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>179</v>
       </c>
@@ -11792,7 +11790,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="35" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>209</v>
       </c>
@@ -11954,7 +11952,7 @@
         <v>73</v>
       </c>
       <c r="BB35" s="35" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="BC35" s="33">
         <v>44890.834027777775</v>
@@ -11963,7 +11961,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="36" spans="1:56" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:56" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>207</v>
       </c>
@@ -12132,7 +12130,7 @@
       </c>
       <c r="BD36"/>
     </row>
-    <row r="37" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>205</v>
       </c>
@@ -12293,7 +12291,7 @@
         <v>73</v>
       </c>
       <c r="BB37" s="35" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="BC37" s="33">
         <v>45180.833333333336</v>
@@ -12302,7 +12300,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="38" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>206</v>
       </c>
@@ -12465,14 +12463,14 @@
       <c r="BB38" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="BC38" s="38">
+      <c r="BC38" s="36">
         <v>44303</v>
       </c>
       <c r="BD38" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="39" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>375</v>
       </c>
@@ -12642,7 +12640,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="40" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>196</v>
       </c>
@@ -12812,7 +12810,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="41" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>200</v>
       </c>
@@ -12983,7 +12981,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="42" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>208</v>
       </c>
@@ -13147,14 +13145,14 @@
       <c r="BB42" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="BC42" s="38">
+      <c r="BC42" s="36">
         <v>44921</v>
       </c>
       <c r="BD42" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="43" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>218</v>
       </c>
@@ -13324,7 +13322,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="44" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>192</v>
       </c>
@@ -13492,7 +13490,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="45" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>210</v>
       </c>
@@ -13659,7 +13657,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="46" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>244</v>
       </c>
@@ -13827,7 +13825,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="47" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>216</v>
       </c>
@@ -13997,7 +13995,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="48" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>211</v>
       </c>
@@ -14165,7 +14163,7 @@
         <v>45096.459363425929</v>
       </c>
     </row>
-    <row r="49" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>214</v>
       </c>
@@ -14329,11 +14327,11 @@
       <c r="BB49" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="BC49" s="38">
+      <c r="BC49" s="36">
         <v>45027</v>
       </c>
     </row>
-    <row r="50" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>212</v>
       </c>
@@ -14501,7 +14499,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="51" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>217</v>
       </c>
@@ -14672,7 +14670,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="52" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>220</v>
       </c>
@@ -14840,7 +14838,7 @@
         <v>44687.458877314813</v>
       </c>
     </row>
-    <row r="53" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>219</v>
       </c>
@@ -15001,7 +14999,7 @@
         <v>73</v>
       </c>
       <c r="BB53" s="35" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="BC53" s="33">
         <v>45182.583333333336</v>
@@ -15010,7 +15008,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="54" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>215</v>
       </c>
@@ -15172,7 +15170,7 @@
         <v>73</v>
       </c>
       <c r="BB54" s="35" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="BC54" s="33">
         <v>44845.70925925926</v>
@@ -15181,7 +15179,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="55" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>213</v>
       </c>
@@ -15344,14 +15342,14 @@
       <c r="BB55" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="BC55" s="39">
+      <c r="BC55" s="37">
         <v>44548</v>
       </c>
       <c r="BD55" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="56" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>311</v>
       </c>
@@ -15518,7 +15516,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="57" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>314</v>
       </c>
@@ -15686,7 +15684,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="58" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>320</v>
       </c>
@@ -15847,13 +15845,13 @@
         <v>73</v>
       </c>
       <c r="BB58" s="35" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="BC58" s="33">
         <v>45219.084027777775</v>
       </c>
     </row>
-    <row r="59" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>323</v>
       </c>
@@ -16020,7 +16018,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="60" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>288</v>
       </c>
@@ -16182,13 +16180,13 @@
         <v>73</v>
       </c>
       <c r="BB60" s="12" t="s">
-        <v>432</v>
-      </c>
-      <c r="BC60" s="38">
+        <v>431</v>
+      </c>
+      <c r="BC60" s="36">
         <v>44602</v>
       </c>
     </row>
-    <row r="61" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>325</v>
       </c>
@@ -16355,7 +16353,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="62" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>328</v>
       </c>
@@ -16516,13 +16514,13 @@
         <v>73</v>
       </c>
       <c r="BB62" s="13" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="BC62" s="33">
         <v>44968.667083333334</v>
       </c>
     </row>
-    <row r="63" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>330</v>
       </c>
@@ -16689,7 +16687,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="64" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>332</v>
       </c>
@@ -16856,7 +16854,7 @@
         <v>45169.710104166668</v>
       </c>
     </row>
-    <row r="65" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>335</v>
       </c>
@@ -17023,7 +17021,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="66" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>338</v>
       </c>
@@ -17186,13 +17184,13 @@
       <c r="BB66" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="BC66" s="38">
+      <c r="BC66" s="36">
         <v>45030</v>
       </c>
     </row>
-    <row r="67" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B67" t="s">
         <v>103</v>
@@ -17207,7 +17205,7 @@
         <v>53</v>
       </c>
       <c r="F67" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G67" s="4">
         <v>8</v>
@@ -17270,7 +17268,7 @@
         <v>104</v>
       </c>
       <c r="AA67" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="AB67" s="1">
         <v>150</v>
@@ -17288,7 +17286,7 @@
         <v>29</v>
       </c>
       <c r="AG67" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="AH67" t="s">
         <v>102</v>
@@ -17303,7 +17301,7 @@
         <v>360</v>
       </c>
       <c r="AL67" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="AM67">
         <v>38.200000000000003</v>
@@ -17352,16 +17350,16 @@
         <v>73</v>
       </c>
       <c r="BB67" s="13" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="BC67" t="s">
         <v>270</v>
       </c>
       <c r="BD67" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
-    <row r="68" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>340</v>
       </c>
@@ -17529,7 +17527,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="69" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>296</v>
       </c>
@@ -17699,7 +17697,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="70" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>299</v>
       </c>
@@ -17869,9 +17867,9 @@
         <v>356</v>
       </c>
     </row>
-    <row r="71" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B71" t="s">
         <v>252</v>
@@ -17886,7 +17884,7 @@
         <v>85</v>
       </c>
       <c r="F71" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G71" s="4">
         <v>9</v>
@@ -17946,7 +17944,7 @@
         <v>-126.59028000000001</v>
       </c>
       <c r="Z71" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="AA71" t="s">
         <v>22</v>
@@ -17961,13 +17959,13 @@
         <v>353</v>
       </c>
       <c r="AE71" t="s">
+        <v>424</v>
+      </c>
+      <c r="AF71" t="s">
         <v>425</v>
       </c>
-      <c r="AF71" t="s">
+      <c r="AG71" t="s">
         <v>426</v>
-      </c>
-      <c r="AG71" t="s">
-        <v>427</v>
       </c>
       <c r="AH71" t="s">
         <v>102</v>
@@ -18036,12 +18034,12 @@
         <v>270</v>
       </c>
     </row>
-    <row r="72" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>399</v>
+      </c>
+      <c r="B72" t="s">
         <v>400</v>
-      </c>
-      <c r="B72" t="s">
-        <v>401</v>
       </c>
       <c r="C72" s="6">
         <v>44985</v>
@@ -18053,7 +18051,7 @@
         <v>182</v>
       </c>
       <c r="F72" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G72" s="4">
         <v>17</v>
@@ -18113,7 +18111,7 @@
         <v>-126.49023</v>
       </c>
       <c r="Z72" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="AA72" t="s">
         <v>22</v>
@@ -18125,16 +18123,16 @@
         <v>80003</v>
       </c>
       <c r="AD72" t="s">
+        <v>401</v>
+      </c>
+      <c r="AE72" t="s">
         <v>402</v>
       </c>
-      <c r="AE72" t="s">
+      <c r="AF72" t="s">
         <v>403</v>
       </c>
-      <c r="AF72" t="s">
+      <c r="AG72" t="s">
         <v>404</v>
-      </c>
-      <c r="AG72" t="s">
-        <v>405</v>
       </c>
       <c r="AH72" t="s">
         <v>31</v>
@@ -18203,9 +18201,9 @@
         <v>270</v>
       </c>
     </row>
-    <row r="73" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B73" t="s">
         <v>108</v>
@@ -18220,7 +18218,7 @@
         <v>159</v>
       </c>
       <c r="F73" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G73" s="4">
         <v>13</v>
@@ -18280,7 +18278,7 @@
         <v>-126.19417</v>
       </c>
       <c r="Z73" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="AA73" t="s">
         <v>22</v>
@@ -18295,13 +18293,13 @@
         <v>146</v>
       </c>
       <c r="AE73" t="s">
+        <v>396</v>
+      </c>
+      <c r="AF73" t="s">
         <v>397</v>
       </c>
-      <c r="AF73" t="s">
+      <c r="AG73" t="s">
         <v>398</v>
-      </c>
-      <c r="AG73" t="s">
-        <v>399</v>
       </c>
       <c r="AH73" t="s">
         <v>31</v>
@@ -18370,7 +18368,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="74" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>302</v>
       </c>
@@ -18541,7 +18539,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="75" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>304</v>
       </c>
@@ -18711,12 +18709,12 @@
         <v>365</v>
       </c>
     </row>
-    <row r="76" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>386</v>
+      </c>
+      <c r="B76" t="s">
         <v>387</v>
-      </c>
-      <c r="B76" t="s">
-        <v>388</v>
       </c>
       <c r="C76" s="6">
         <v>44956</v>
@@ -18725,10 +18723,10 @@
         <v>2</v>
       </c>
       <c r="E76" t="s">
+        <v>388</v>
+      </c>
+      <c r="F76" t="s">
         <v>389</v>
-      </c>
-      <c r="F76" t="s">
-        <v>390</v>
       </c>
       <c r="G76" s="4">
         <v>15</v>
@@ -18788,7 +18786,7 @@
         <v>-126.13715000000001</v>
       </c>
       <c r="Z76" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="AA76" t="s">
         <v>22</v>
@@ -18803,13 +18801,13 @@
         <v>146</v>
       </c>
       <c r="AE76" t="s">
+        <v>390</v>
+      </c>
+      <c r="AF76" t="s">
         <v>391</v>
       </c>
-      <c r="AF76" t="s">
-        <v>392</v>
-      </c>
       <c r="AG76" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AH76" t="s">
         <v>102</v>
@@ -18878,7 +18876,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="77" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>307</v>
       </c>
@@ -19039,13 +19037,13 @@
         <v>73</v>
       </c>
       <c r="BB77" s="35" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="BC77" s="33">
         <v>44944.335092592592</v>
       </c>
     </row>
-    <row r="78" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>366</v>
       </c>
@@ -19212,12 +19210,12 @@
         <v>270</v>
       </c>
     </row>
-    <row r="79" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>477</v>
+      </c>
+      <c r="B79" t="s">
         <v>478</v>
-      </c>
-      <c r="B79" t="s">
-        <v>479</v>
       </c>
       <c r="C79" s="6">
         <v>44953</v>
@@ -19226,10 +19224,10 @@
         <v>5</v>
       </c>
       <c r="E79" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F79" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G79" s="4">
         <v>17</v>
@@ -19289,10 +19287,10 @@
         <v>-125.75945</v>
       </c>
       <c r="Z79" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AA79" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="AB79" s="1">
         <v>150.26</v>
@@ -19304,10 +19302,10 @@
         <v>225</v>
       </c>
       <c r="AE79" t="s">
+        <v>481</v>
+      </c>
+      <c r="AF79" t="s">
         <v>482</v>
-      </c>
-      <c r="AF79" t="s">
-        <v>483</v>
       </c>
       <c r="AG79" t="s">
         <v>103</v>
@@ -19316,7 +19314,7 @@
         <v>31</v>
       </c>
       <c r="AI79" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="AJ79" t="s">
         <v>76</v>
@@ -19325,7 +19323,7 @@
         <v>360</v>
       </c>
       <c r="AL79" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="AM79">
         <v>38</v>
@@ -19372,19 +19370,19 @@
       <c r="BA79" t="s">
         <v>73</v>
       </c>
-      <c r="BB79" s="37" t="s">
-        <v>484</v>
+      <c r="BB79" s="8" t="s">
+        <v>483</v>
       </c>
       <c r="BC79" s="33">
         <v>45336.959664351853</v>
       </c>
       <c r="BD79" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
-    <row r="80" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B80" t="s">
         <v>84</v>
@@ -19459,7 +19457,7 @@
         <v>-125.67333000000001</v>
       </c>
       <c r="Z80" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="AA80" t="s">
         <v>22</v>
@@ -19471,16 +19469,16 @@
         <v>85132</v>
       </c>
       <c r="AD80" t="s">
+        <v>413</v>
+      </c>
+      <c r="AE80" t="s">
         <v>414</v>
       </c>
-      <c r="AE80" t="s">
+      <c r="AF80" t="s">
         <v>415</v>
       </c>
-      <c r="AF80" t="s">
+      <c r="AG80" t="s">
         <v>416</v>
-      </c>
-      <c r="AG80" t="s">
-        <v>417</v>
       </c>
       <c r="AH80" t="s">
         <v>31</v>
@@ -19549,9 +19547,9 @@
         <v>270</v>
       </c>
     </row>
-    <row r="81" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B81" t="s">
         <v>133</v>
@@ -19563,10 +19561,10 @@
         <v>225</v>
       </c>
       <c r="E81" t="s">
+        <v>406</v>
+      </c>
+      <c r="F81" t="s">
         <v>407</v>
-      </c>
-      <c r="F81" t="s">
-        <v>408</v>
       </c>
       <c r="G81" s="4">
         <v>11</v>
@@ -19626,7 +19624,7 @@
         <v>-126.08373</v>
       </c>
       <c r="Z81" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="AA81" s="20" t="s">
         <v>22</v>
@@ -19638,16 +19636,16 @@
         <v>85133</v>
       </c>
       <c r="AD81" t="s">
+        <v>408</v>
+      </c>
+      <c r="AE81" t="s">
         <v>409</v>
       </c>
-      <c r="AE81" t="s">
+      <c r="AF81" t="s">
         <v>410</v>
       </c>
-      <c r="AF81" t="s">
+      <c r="AG81" t="s">
         <v>411</v>
-      </c>
-      <c r="AG81" t="s">
-        <v>412</v>
       </c>
       <c r="AH81" t="s">
         <v>31</v>
@@ -19716,9 +19714,9 @@
         <v>270</v>
       </c>
     </row>
-    <row r="82" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B82" t="s">
         <v>133</v>
@@ -19733,7 +19731,7 @@
         <v>53</v>
       </c>
       <c r="F82" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G82" s="4">
         <v>7</v>
@@ -19793,10 +19791,10 @@
         <v>-126.125421</v>
       </c>
       <c r="Z82" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="AA82" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="AB82" s="1">
         <v>150.01</v>
@@ -19808,13 +19806,13 @@
         <v>225</v>
       </c>
       <c r="AE82" t="s">
+        <v>454</v>
+      </c>
+      <c r="AF82" t="s">
         <v>455</v>
       </c>
-      <c r="AF82" t="s">
+      <c r="AG82" t="s">
         <v>456</v>
-      </c>
-      <c r="AG82" t="s">
-        <v>457</v>
       </c>
       <c r="AH82" t="s">
         <v>31</v>
@@ -19829,7 +19827,7 @@
         <v>360</v>
       </c>
       <c r="AL82" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="AM82">
         <v>39.799999999999997</v>
@@ -19883,12 +19881,12 @@
         <v>270</v>
       </c>
     </row>
-    <row r="83" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>447</v>
+      </c>
+      <c r="B83" t="s">
         <v>448</v>
-      </c>
-      <c r="B83" t="s">
-        <v>449</v>
       </c>
       <c r="C83" s="6">
         <v>45327</v>
@@ -19900,7 +19898,7 @@
         <v>53</v>
       </c>
       <c r="F83" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G83" s="4">
         <v>10</v>
@@ -19960,10 +19958,10 @@
         <v>-126.54429</v>
       </c>
       <c r="Z83" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="AA83" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="AB83" s="1">
         <v>150.03</v>
@@ -19972,16 +19970,16 @@
         <v>94433</v>
       </c>
       <c r="AD83" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="AE83" t="s">
+        <v>449</v>
+      </c>
+      <c r="AF83" t="s">
         <v>450</v>
       </c>
-      <c r="AF83" t="s">
+      <c r="AG83" t="s">
         <v>451</v>
-      </c>
-      <c r="AG83" t="s">
-        <v>452</v>
       </c>
       <c r="AH83" t="s">
         <v>31</v>
@@ -19996,7 +19994,7 @@
         <v>62</v>
       </c>
       <c r="AL83" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="AM83">
         <v>39.4</v>
@@ -20050,9 +20048,9 @@
         <v>270</v>
       </c>
     </row>
-    <row r="84" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B84" t="s">
         <v>84</v>
@@ -20067,7 +20065,7 @@
         <v>53</v>
       </c>
       <c r="F84" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G84" s="4">
         <v>28</v>
@@ -20127,10 +20125,10 @@
         <v>-125.72008</v>
       </c>
       <c r="Z84" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="AA84" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="AB84" s="1">
         <v>150.09</v>
@@ -20142,13 +20140,13 @@
         <v>225</v>
       </c>
       <c r="AE84" t="s">
+        <v>459</v>
+      </c>
+      <c r="AF84" t="s">
         <v>460</v>
       </c>
-      <c r="AF84" t="s">
-        <v>461</v>
-      </c>
       <c r="AG84" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="AH84" t="s">
         <v>31</v>
@@ -20217,12 +20215,12 @@
         <v>270</v>
       </c>
       <c r="BD84" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
-    <row r="85" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B85" t="s">
         <v>232</v>
@@ -20237,7 +20235,7 @@
         <v>53</v>
       </c>
       <c r="F85" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G85" s="4">
         <v>5</v>
@@ -20297,10 +20295,10 @@
         <v>-126.16364299999999</v>
       </c>
       <c r="Z85" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="AA85" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="AB85" s="1">
         <v>150.22999999999999</v>
@@ -20309,16 +20307,16 @@
         <v>94437</v>
       </c>
       <c r="AD85" t="s">
+        <v>438</v>
+      </c>
+      <c r="AE85" t="s">
         <v>439</v>
       </c>
-      <c r="AE85" t="s">
+      <c r="AF85" t="s">
         <v>440</v>
       </c>
-      <c r="AF85" t="s">
+      <c r="AG85" t="s">
         <v>441</v>
-      </c>
-      <c r="AG85" t="s">
-        <v>442</v>
       </c>
       <c r="AH85" t="s">
         <v>31</v>
@@ -20333,7 +20331,7 @@
         <v>62</v>
       </c>
       <c r="AL85" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="AM85">
         <v>38.700000000000003</v>
@@ -20388,9 +20386,9 @@
         <v>270</v>
       </c>
     </row>
-    <row r="86" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B86" t="s">
         <v>84</v>
@@ -20405,7 +20403,7 @@
         <v>53</v>
       </c>
       <c r="F86" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G86" s="4">
         <v>3</v>
@@ -20465,10 +20463,10 @@
         <v>-125.618487</v>
       </c>
       <c r="Z86" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="AA86" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="AB86" s="1">
         <v>150.5</v>
@@ -20480,13 +20478,13 @@
         <v>225</v>
       </c>
       <c r="AE86" t="s">
+        <v>464</v>
+      </c>
+      <c r="AF86" t="s">
         <v>465</v>
       </c>
-      <c r="AF86" t="s">
+      <c r="AG86" t="s">
         <v>466</v>
-      </c>
-      <c r="AG86" t="s">
-        <v>467</v>
       </c>
       <c r="AH86" t="s">
         <v>31</v>
@@ -20501,7 +20499,7 @@
         <v>360</v>
       </c>
       <c r="AL86" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="AM86">
         <v>38.299999999999997</v>
@@ -20575,18 +20573,18 @@
       <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.5546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" style="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.5546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.44140625" style="23" customWidth="1"/>
-    <col min="8" max="16384" width="14.33203125" style="23"/>
+    <col min="4" max="4" width="10.7109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.5703125" style="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" style="23" customWidth="1"/>
+    <col min="8" max="16384" width="14.28515625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
         <v>376</v>
       </c>
@@ -20609,7 +20607,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
         <v>55</v>
       </c>
@@ -20632,7 +20630,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
         <v>74</v>
       </c>
@@ -20655,7 +20653,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>58</v>
       </c>
@@ -20678,7 +20676,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
         <v>71</v>
       </c>
@@ -20701,10 +20699,10 @@
         <v>269</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
         <v>64</v>
       </c>
@@ -20727,7 +20725,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
         <v>20</v>
       </c>
@@ -20750,7 +20748,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
         <v>80</v>
       </c>
@@ -20773,7 +20771,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
         <v>167</v>
       </c>
@@ -20796,7 +20794,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
         <v>160</v>
       </c>
@@ -20819,7 +20817,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
         <v>151</v>
       </c>
@@ -20842,7 +20840,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
         <v>100</v>
       </c>
@@ -20865,7 +20863,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
         <v>104</v>
       </c>
@@ -20885,10 +20883,10 @@
         <v>29</v>
       </c>
       <c r="G13" s="28" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
         <v>97</v>
       </c>
@@ -20911,7 +20909,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
         <v>156</v>
       </c>
@@ -20934,7 +20932,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
         <v>136</v>
       </c>
@@ -20957,7 +20955,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
         <v>120</v>
       </c>
@@ -20980,7 +20978,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
         <v>127</v>
       </c>
@@ -21003,10 +21001,10 @@
         <v>269</v>
       </c>
       <c r="H18" s="23" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
         <v>164</v>
       </c>
@@ -21029,7 +21027,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
         <v>123</v>
       </c>
@@ -21052,7 +21050,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
         <v>116</v>
       </c>
@@ -21075,7 +21073,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
         <v>111</v>
       </c>
@@ -21098,7 +21096,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="29" t="s">
         <v>131</v>
       </c>
@@ -21121,7 +21119,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="23" t="s">
         <v>90</v>
       </c>
@@ -21144,7 +21142,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="23" t="s">
         <v>172</v>
       </c>
@@ -21164,10 +21162,10 @@
         <v>173</v>
       </c>
       <c r="G25" s="28" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="23" t="s">
         <v>187</v>
       </c>
@@ -21190,7 +21188,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="23" t="s">
         <v>196</v>
       </c>
@@ -21213,7 +21211,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="23" t="s">
         <v>207</v>
       </c>
@@ -21236,7 +21234,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="23" t="s">
         <v>190</v>
       </c>
@@ -21259,7 +21257,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="23" t="s">
         <v>205</v>
       </c>
@@ -21282,7 +21280,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="23" t="s">
         <v>206</v>
       </c>
@@ -21305,7 +21303,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="23" t="s">
         <v>217</v>
       </c>
@@ -21328,10 +21326,10 @@
         <v>269</v>
       </c>
       <c r="H32" s="23" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="23" t="s">
         <v>218</v>
       </c>
@@ -21354,7 +21352,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="23" t="s">
         <v>176</v>
       </c>
@@ -21377,7 +21375,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="23" t="s">
         <v>179</v>
       </c>
@@ -21400,7 +21398,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="23" t="s">
         <v>211</v>
       </c>
@@ -21423,7 +21421,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="23" t="s">
         <v>219</v>
       </c>
@@ -21446,7 +21444,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="23" t="s">
         <v>192</v>
       </c>
@@ -21469,7 +21467,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="23" t="s">
         <v>214</v>
       </c>
@@ -21492,7 +21490,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="23" t="s">
         <v>183</v>
       </c>
@@ -21515,7 +21513,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="23" t="s">
         <v>200</v>
       </c>
@@ -21538,7 +21536,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="23" t="s">
         <v>220</v>
       </c>
@@ -21561,7 +21559,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="23" t="s">
         <v>215</v>
       </c>
@@ -21584,10 +21582,10 @@
         <v>269</v>
       </c>
       <c r="H43" s="23" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="23" t="s">
         <v>208</v>
       </c>
@@ -21607,10 +21605,10 @@
         <v>233</v>
       </c>
       <c r="G44" s="25" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="23" t="s">
         <v>210</v>
       </c>
@@ -21633,7 +21631,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="23" t="s">
         <v>209</v>
       </c>
@@ -21656,10 +21654,10 @@
         <v>269</v>
       </c>
       <c r="H46" s="23" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="23" t="s">
         <v>216</v>
       </c>
@@ -21682,7 +21680,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="23" t="s">
         <v>212</v>
       </c>
@@ -21705,7 +21703,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="23" t="s">
         <v>213</v>
       </c>
@@ -21728,7 +21726,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="23" t="s">
         <v>244</v>
       </c>
@@ -21751,7 +21749,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="23" t="s">
         <v>330</v>
       </c>
@@ -21774,7 +21772,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="23" t="s">
         <v>340</v>
       </c>
@@ -21797,7 +21795,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="29" t="s">
         <v>375</v>
       </c>
@@ -21820,7 +21818,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="23" t="s">
         <v>296</v>
       </c>
@@ -21843,7 +21841,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="23" t="s">
         <v>302</v>
       </c>
@@ -21866,7 +21864,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="23" t="s">
         <v>323</v>
       </c>
@@ -21889,7 +21887,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="23" t="s">
         <v>288</v>
       </c>
@@ -21912,7 +21910,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="23" t="s">
         <v>328</v>
       </c>
@@ -21935,7 +21933,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="23" t="s">
         <v>325</v>
       </c>
@@ -21955,10 +21953,10 @@
         <v>327</v>
       </c>
       <c r="G59" s="28" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="23" t="s">
         <v>299</v>
       </c>
@@ -21981,7 +21979,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="23" t="s">
         <v>332</v>
       </c>
@@ -22004,7 +22002,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="23" t="s">
         <v>366</v>
       </c>
@@ -22027,7 +22025,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="23" t="s">
         <v>304</v>
       </c>
@@ -22050,7 +22048,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="23" t="s">
         <v>314</v>
       </c>
@@ -22073,7 +22071,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="23" t="s">
         <v>307</v>
       </c>
@@ -22096,10 +22094,10 @@
         <v>269</v>
       </c>
       <c r="H65" s="23" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="23" t="s">
         <v>335</v>
       </c>
@@ -22122,7 +22120,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="23" t="s">
         <v>311</v>
       </c>
@@ -22142,10 +22140,10 @@
         <v>313</v>
       </c>
       <c r="G67" s="28" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="23" t="s">
         <v>320</v>
       </c>
@@ -22168,7 +22166,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="23" t="s">
         <v>291</v>
       </c>
@@ -22188,10 +22186,10 @@
         <v>293</v>
       </c>
       <c r="G69" s="28" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="23" t="s">
         <v>338</v>
       </c>
@@ -22229,20 +22227,20 @@
       <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="10.33203125" customWidth="1"/>
-    <col min="9" max="9" width="60.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="41.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="124.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="60.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="124.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>265</v>
       </c>
@@ -22266,7 +22264,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -22300,7 +22298,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -22337,7 +22335,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -22374,7 +22372,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -22411,7 +22409,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>71</v>
       </c>
@@ -22445,7 +22443,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>74</v>
       </c>
@@ -22482,7 +22480,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>80</v>
       </c>
@@ -22519,7 +22517,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>104</v>
       </c>
@@ -22556,7 +22554,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>90</v>
       </c>
@@ -22593,7 +22591,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>100</v>
       </c>
@@ -22627,7 +22625,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>97</v>
       </c>
@@ -22661,7 +22659,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>111</v>
       </c>
@@ -22695,7 +22693,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>131</v>
       </c>
@@ -22727,7 +22725,7 @@
       </c>
       <c r="J14" s="15"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>116</v>
       </c>
@@ -22764,7 +22762,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>127</v>
       </c>
@@ -22801,7 +22799,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>123</v>
       </c>
@@ -22838,7 +22836,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>120</v>
       </c>
@@ -22875,7 +22873,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>151</v>
       </c>
@@ -22912,7 +22910,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>136</v>
       </c>
@@ -22949,7 +22947,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>156</v>
       </c>
@@ -22986,7 +22984,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>160</v>
       </c>
@@ -23020,7 +23018,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>167</v>
       </c>
@@ -23057,7 +23055,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>164</v>
       </c>
@@ -23094,7 +23092,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>183</v>
       </c>
@@ -23131,7 +23129,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>176</v>
       </c>
@@ -23165,7 +23163,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>179</v>
       </c>
@@ -23202,7 +23200,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>187</v>
       </c>
@@ -23239,7 +23237,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>190</v>
       </c>
@@ -23273,7 +23271,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>192</v>
       </c>
@@ -23307,7 +23305,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>172</v>
       </c>
@@ -23344,7 +23342,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>196</v>
       </c>
@@ -23381,7 +23379,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>205</v>
       </c>
@@ -23418,7 +23416,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>206</v>
       </c>
@@ -23455,7 +23453,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>200</v>
       </c>
@@ -23492,7 +23490,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>209</v>
       </c>
@@ -23529,7 +23527,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>207</v>
       </c>
@@ -23563,7 +23561,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>208</v>
       </c>
@@ -23600,7 +23598,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>210</v>
       </c>
@@ -23634,7 +23632,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>218</v>
       </c>
@@ -23671,7 +23669,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>217</v>
       </c>
@@ -23708,7 +23706,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>220</v>
       </c>
@@ -23742,7 +23740,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>219</v>
       </c>
@@ -23779,7 +23777,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>216</v>
       </c>
@@ -23816,7 +23814,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>214</v>
       </c>
@@ -23850,7 +23848,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>215</v>
       </c>
@@ -23887,7 +23885,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>244</v>
       </c>
@@ -23921,7 +23919,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>211</v>
       </c>
@@ -23955,7 +23953,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>212</v>
       </c>
@@ -23989,7 +23987,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>213</v>
       </c>
@@ -24026,7 +24024,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>288</v>
       </c>
@@ -24060,7 +24058,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>323</v>
       </c>
@@ -24094,7 +24092,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>325</v>
       </c>
@@ -24128,7 +24126,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>338</v>
       </c>
@@ -24162,7 +24160,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>294</v>
       </c>
@@ -24196,7 +24194,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>328</v>
       </c>
@@ -24230,7 +24228,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>330</v>
       </c>
@@ -24264,7 +24262,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>340</v>
       </c>
@@ -24298,7 +24296,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>320</v>
       </c>
@@ -24332,7 +24330,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>332</v>
       </c>
@@ -24366,7 +24364,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>335</v>
       </c>
@@ -24400,7 +24398,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>302</v>
       </c>
@@ -24434,7 +24432,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>311</v>
       </c>
@@ -24468,7 +24466,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>314</v>
       </c>
@@ -24502,7 +24500,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>304</v>
       </c>
@@ -24536,7 +24534,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>307</v>
       </c>
@@ -24570,7 +24568,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>225</v>
       </c>
@@ -24604,7 +24602,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>291</v>
       </c>
@@ -24638,7 +24636,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>296</v>
       </c>
@@ -24672,7 +24670,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>299</v>
       </c>
@@ -24723,104 +24721,104 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>225</v>
       </c>

</xml_diff>